<commit_message>
revise CDA from 2T to 4T
</commit_message>
<xml_diff>
--- a/calc05unit.xlsx
+++ b/calc05unit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yubis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FFEB9F-1D5E-43A0-A6A0-7323ECC2066A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF7C19C-4CFE-4703-8860-8D8AD322BBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" xr2:uid="{9B936CDB-E232-41AF-B13E-06C799A84B33}"/>
   </bookViews>
@@ -1099,7 +1099,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1196,22 +1196,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1223,8 +1214,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1542,7 +1566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9F458F-CFA5-4071-8A17-F710DFFAE914}">
   <dimension ref="A1:NB2409"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1561,7 +1587,7 @@
   <sheetData>
     <row r="1" spans="1:366" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C1" s="20"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="32" t="s">
         <v>82</v>
       </c>
       <c r="E1" s="15"/>
@@ -1588,7 +1614,7 @@
       <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1663,10 +1689,10 @@
       <c r="BF2"/>
     </row>
     <row r="3" spans="1:366" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1742,8 +1768,8 @@
       <c r="BF3"/>
     </row>
     <row r="4" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="26" t="s">
         <v>12</v>
       </c>
@@ -2127,10 +2153,10 @@
       <c r="NB4"/>
     </row>
     <row r="5" spans="1:366" s="9" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="27" t="s">
         <v>1</v>
       </c>
@@ -2505,10 +2531,10 @@
       <c r="NB5"/>
     </row>
     <row r="6" spans="1:366" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="38" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -2880,8 +2906,8 @@
       <c r="NB6"/>
     </row>
     <row r="7" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="22" t="s">
         <v>18</v>
       </c>
@@ -2895,8 +2921,8 @@
       <c r="L7"/>
     </row>
     <row r="8" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="22" t="s">
         <v>29</v>
       </c>
@@ -2910,8 +2936,8 @@
       <c r="L8"/>
     </row>
     <row r="9" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="26" t="s">
         <v>13</v>
       </c>
@@ -3282,8 +3308,8 @@
       <c r="NB9"/>
     </row>
     <row r="10" spans="1:366" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="33"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="38" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="20" t="s">
@@ -3658,8 +3684,8 @@
       <c r="NB10"/>
     </row>
     <row r="11" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="22" t="s">
         <v>24</v>
       </c>
@@ -3668,8 +3694,8 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="22" t="s">
         <v>14</v>
       </c>
@@ -3677,853 +3703,853 @@
       <c r="J12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="22" t="s">
+    <row r="13" spans="1:366" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="21"/>
       <c r="J13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="19"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
+    <row r="14" spans="1:366" x14ac:dyDescent="0.4">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="28"/>
       <c r="J14"/>
-      <c r="K14"/>
       <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
-      <c r="AE14"/>
-      <c r="AF14"/>
-      <c r="AG14"/>
-      <c r="AH14"/>
-      <c r="AI14"/>
-      <c r="AJ14"/>
-      <c r="AK14"/>
-      <c r="AL14"/>
-      <c r="AM14"/>
-      <c r="AN14"/>
-      <c r="AO14"/>
-      <c r="AP14"/>
-      <c r="AQ14"/>
-      <c r="AR14"/>
-      <c r="AS14"/>
-      <c r="AT14"/>
-      <c r="AU14"/>
-      <c r="AV14"/>
-      <c r="AW14"/>
-      <c r="AX14"/>
-      <c r="AY14"/>
-      <c r="AZ14"/>
-      <c r="BA14"/>
-      <c r="BB14"/>
-      <c r="BC14"/>
-      <c r="BD14"/>
-      <c r="BE14"/>
-      <c r="BF14"/>
-      <c r="BG14"/>
-      <c r="BH14"/>
-      <c r="BI14"/>
-      <c r="BJ14"/>
-      <c r="BK14"/>
-      <c r="BL14"/>
-      <c r="BM14"/>
-      <c r="BN14"/>
-      <c r="BO14"/>
-      <c r="BP14"/>
-      <c r="BQ14"/>
-      <c r="BR14"/>
-      <c r="BS14"/>
-      <c r="BT14"/>
-      <c r="BU14"/>
-      <c r="BV14"/>
-      <c r="BW14"/>
-      <c r="BX14"/>
-      <c r="BY14"/>
-      <c r="BZ14"/>
-      <c r="CA14"/>
-      <c r="CB14"/>
-      <c r="CC14"/>
-      <c r="CD14"/>
-      <c r="CE14"/>
-      <c r="CF14"/>
-      <c r="CG14"/>
-      <c r="CH14"/>
-      <c r="CI14"/>
-      <c r="CJ14"/>
-      <c r="CK14"/>
-      <c r="CL14"/>
-      <c r="CM14"/>
-      <c r="CN14"/>
-      <c r="CO14"/>
-      <c r="CP14"/>
-      <c r="CQ14"/>
-      <c r="CR14"/>
-      <c r="CS14"/>
-      <c r="CT14"/>
-      <c r="CU14"/>
-      <c r="CV14"/>
-      <c r="CW14"/>
-      <c r="CX14"/>
-      <c r="CY14"/>
-      <c r="CZ14"/>
-      <c r="DA14"/>
-      <c r="DB14"/>
-      <c r="DC14"/>
-      <c r="DD14"/>
-      <c r="DE14"/>
-      <c r="DF14"/>
-      <c r="DG14"/>
-      <c r="DH14"/>
-      <c r="DI14"/>
-      <c r="DJ14"/>
-      <c r="DK14"/>
-      <c r="DL14"/>
-      <c r="DM14"/>
-      <c r="DN14"/>
-      <c r="DO14"/>
-      <c r="DP14"/>
-      <c r="DQ14"/>
-      <c r="DR14"/>
-      <c r="DS14"/>
-      <c r="DT14"/>
-      <c r="DU14"/>
-      <c r="DV14"/>
-      <c r="DW14"/>
-      <c r="DX14"/>
-      <c r="DY14"/>
-      <c r="DZ14"/>
-      <c r="EA14"/>
-      <c r="EB14"/>
-      <c r="EC14"/>
-      <c r="ED14"/>
-      <c r="EE14"/>
-      <c r="EF14"/>
-      <c r="EG14"/>
-      <c r="EH14"/>
-      <c r="EI14"/>
-      <c r="EJ14"/>
-      <c r="EK14"/>
-      <c r="EL14"/>
-      <c r="EM14"/>
-      <c r="EN14"/>
-      <c r="EO14"/>
-      <c r="EP14"/>
-      <c r="EQ14"/>
-      <c r="ER14"/>
-      <c r="ES14"/>
-      <c r="ET14"/>
-      <c r="EU14"/>
-      <c r="EV14"/>
-      <c r="EW14"/>
-      <c r="EX14"/>
-      <c r="EY14"/>
-      <c r="EZ14"/>
-      <c r="FA14"/>
-      <c r="FB14"/>
-      <c r="FC14"/>
-      <c r="FD14"/>
-      <c r="FE14"/>
-      <c r="FF14"/>
-      <c r="FG14"/>
-      <c r="FH14"/>
-      <c r="FI14"/>
-      <c r="FJ14"/>
-      <c r="FK14"/>
-      <c r="FL14"/>
-      <c r="FM14"/>
-      <c r="FN14"/>
-      <c r="FO14"/>
-      <c r="FP14"/>
-      <c r="FQ14"/>
-      <c r="FR14"/>
-      <c r="FS14"/>
-      <c r="FT14"/>
-      <c r="FU14"/>
-      <c r="FV14"/>
-      <c r="FW14"/>
-      <c r="FX14"/>
-      <c r="FY14"/>
-      <c r="FZ14"/>
-      <c r="GA14"/>
-      <c r="GB14"/>
-      <c r="GC14"/>
-      <c r="GD14"/>
-      <c r="GE14"/>
-      <c r="GF14"/>
-      <c r="GG14"/>
-      <c r="GH14"/>
-      <c r="GI14"/>
-      <c r="GJ14"/>
-      <c r="GK14"/>
-      <c r="GL14"/>
-      <c r="GM14"/>
-      <c r="GN14"/>
-      <c r="GO14"/>
-      <c r="GP14"/>
-      <c r="GQ14"/>
-      <c r="GR14"/>
-      <c r="GS14"/>
-      <c r="GT14"/>
-      <c r="GU14"/>
-      <c r="GV14"/>
-      <c r="GW14"/>
-      <c r="GX14"/>
-      <c r="GY14"/>
-      <c r="GZ14"/>
-      <c r="HA14"/>
-      <c r="HB14"/>
-      <c r="HC14"/>
-      <c r="HD14"/>
-      <c r="HE14"/>
-      <c r="HF14"/>
-      <c r="HG14"/>
-      <c r="HH14"/>
-      <c r="HI14"/>
-      <c r="HJ14"/>
-      <c r="HK14"/>
-      <c r="HL14"/>
-      <c r="HM14"/>
-      <c r="HN14"/>
-      <c r="HO14"/>
-      <c r="HP14"/>
-      <c r="HQ14"/>
-      <c r="HR14"/>
-      <c r="HS14"/>
-      <c r="HT14"/>
-      <c r="HU14"/>
-      <c r="HV14"/>
-      <c r="HW14"/>
-      <c r="HX14"/>
-      <c r="HY14"/>
-      <c r="HZ14"/>
-      <c r="IA14"/>
-      <c r="IB14"/>
-      <c r="IC14"/>
-      <c r="ID14"/>
-      <c r="IE14"/>
-      <c r="IF14"/>
-      <c r="IG14"/>
-      <c r="IH14"/>
-      <c r="II14"/>
-      <c r="IJ14"/>
-      <c r="IK14"/>
-      <c r="IL14"/>
-      <c r="IM14"/>
-      <c r="IN14"/>
-      <c r="IO14"/>
-      <c r="IP14"/>
-      <c r="IQ14"/>
-      <c r="IR14"/>
-      <c r="IS14"/>
-      <c r="IT14"/>
-      <c r="IU14"/>
-      <c r="IV14"/>
-      <c r="IW14"/>
-      <c r="IX14"/>
-      <c r="IY14"/>
-      <c r="IZ14"/>
-      <c r="JA14"/>
-      <c r="JB14"/>
-      <c r="JC14"/>
-      <c r="JD14"/>
-      <c r="JE14"/>
-      <c r="JF14"/>
-      <c r="JG14"/>
-      <c r="JH14"/>
-      <c r="JI14"/>
-      <c r="JJ14"/>
-      <c r="JK14"/>
-      <c r="JL14"/>
-      <c r="JM14"/>
-      <c r="JN14"/>
-      <c r="JO14"/>
-      <c r="JP14"/>
-      <c r="JQ14"/>
-      <c r="JR14"/>
-      <c r="JS14"/>
-      <c r="JT14"/>
-      <c r="JU14"/>
-      <c r="JV14"/>
-      <c r="JW14"/>
-      <c r="JX14"/>
-      <c r="JY14"/>
-      <c r="JZ14"/>
-      <c r="KA14"/>
-      <c r="KB14"/>
-      <c r="KC14"/>
-      <c r="KD14"/>
-      <c r="KE14"/>
-      <c r="KF14"/>
-      <c r="KG14"/>
-      <c r="KH14"/>
-      <c r="KI14"/>
-      <c r="KJ14"/>
-      <c r="KK14"/>
-      <c r="KL14"/>
-      <c r="KM14"/>
-      <c r="KN14"/>
-      <c r="KO14"/>
-      <c r="KP14"/>
-      <c r="KQ14"/>
-      <c r="KR14"/>
-      <c r="KS14"/>
-      <c r="KT14"/>
-      <c r="KU14"/>
-      <c r="KV14"/>
-      <c r="KW14"/>
-      <c r="KX14"/>
-      <c r="KY14"/>
-      <c r="KZ14"/>
-      <c r="LA14"/>
-      <c r="LB14"/>
-      <c r="LC14"/>
-      <c r="LD14"/>
-      <c r="LE14"/>
-      <c r="LF14"/>
-      <c r="LG14"/>
-      <c r="LH14"/>
-      <c r="LI14"/>
-      <c r="LJ14"/>
-      <c r="LK14"/>
-      <c r="LL14"/>
-      <c r="LM14"/>
-      <c r="LN14"/>
-      <c r="LO14"/>
-      <c r="LP14"/>
-      <c r="LQ14"/>
-      <c r="LR14"/>
-      <c r="LS14"/>
-      <c r="LT14"/>
-      <c r="LU14"/>
-      <c r="LV14"/>
-      <c r="LW14"/>
-      <c r="LX14"/>
-      <c r="LY14"/>
-      <c r="LZ14"/>
-      <c r="MA14"/>
-      <c r="MB14"/>
-      <c r="MC14"/>
-      <c r="MD14"/>
-      <c r="ME14"/>
-      <c r="MF14"/>
-      <c r="MG14"/>
-      <c r="MH14"/>
-      <c r="MI14"/>
-      <c r="MJ14"/>
-      <c r="MK14"/>
-      <c r="ML14"/>
-      <c r="MM14"/>
-      <c r="MN14"/>
-      <c r="MO14"/>
-      <c r="MP14"/>
-      <c r="MQ14"/>
-      <c r="MR14"/>
-      <c r="MS14"/>
-      <c r="MT14"/>
-      <c r="MU14"/>
-      <c r="MV14"/>
-      <c r="MW14"/>
-      <c r="MX14"/>
-      <c r="MY14"/>
-      <c r="MZ14"/>
-      <c r="NA14"/>
-      <c r="NB14"/>
     </row>
     <row r="15" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A15" s="33"/>
-      <c r="B15" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" s="28"/>
       <c r="J15"/>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="22" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D16" s="28"/>
       <c r="J16"/>
       <c r="L16"/>
     </row>
     <row r="17" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="22" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D17" s="28"/>
       <c r="J17"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D18" s="28"/>
       <c r="J18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+    <row r="19" spans="1:366" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="39"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="22" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D19" s="28"/>
       <c r="J19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:366" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="28"/>
+    <row r="20" spans="1:366" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="39"/>
+      <c r="B20" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="19"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
       <c r="J20"/>
+      <c r="K20"/>
       <c r="L20"/>
-    </row>
-    <row r="21" spans="1:366" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="33"/>
-      <c r="B21" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="19"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
+      <c r="BU20"/>
+      <c r="BV20"/>
+      <c r="BW20"/>
+      <c r="BX20"/>
+      <c r="BY20"/>
+      <c r="BZ20"/>
+      <c r="CA20"/>
+      <c r="CB20"/>
+      <c r="CC20"/>
+      <c r="CD20"/>
+      <c r="CE20"/>
+      <c r="CF20"/>
+      <c r="CG20"/>
+      <c r="CH20"/>
+      <c r="CI20"/>
+      <c r="CJ20"/>
+      <c r="CK20"/>
+      <c r="CL20"/>
+      <c r="CM20"/>
+      <c r="CN20"/>
+      <c r="CO20"/>
+      <c r="CP20"/>
+      <c r="CQ20"/>
+      <c r="CR20"/>
+      <c r="CS20"/>
+      <c r="CT20"/>
+      <c r="CU20"/>
+      <c r="CV20"/>
+      <c r="CW20"/>
+      <c r="CX20"/>
+      <c r="CY20"/>
+      <c r="CZ20"/>
+      <c r="DA20"/>
+      <c r="DB20"/>
+      <c r="DC20"/>
+      <c r="DD20"/>
+      <c r="DE20"/>
+      <c r="DF20"/>
+      <c r="DG20"/>
+      <c r="DH20"/>
+      <c r="DI20"/>
+      <c r="DJ20"/>
+      <c r="DK20"/>
+      <c r="DL20"/>
+      <c r="DM20"/>
+      <c r="DN20"/>
+      <c r="DO20"/>
+      <c r="DP20"/>
+      <c r="DQ20"/>
+      <c r="DR20"/>
+      <c r="DS20"/>
+      <c r="DT20"/>
+      <c r="DU20"/>
+      <c r="DV20"/>
+      <c r="DW20"/>
+      <c r="DX20"/>
+      <c r="DY20"/>
+      <c r="DZ20"/>
+      <c r="EA20"/>
+      <c r="EB20"/>
+      <c r="EC20"/>
+      <c r="ED20"/>
+      <c r="EE20"/>
+      <c r="EF20"/>
+      <c r="EG20"/>
+      <c r="EH20"/>
+      <c r="EI20"/>
+      <c r="EJ20"/>
+      <c r="EK20"/>
+      <c r="EL20"/>
+      <c r="EM20"/>
+      <c r="EN20"/>
+      <c r="EO20"/>
+      <c r="EP20"/>
+      <c r="EQ20"/>
+      <c r="ER20"/>
+      <c r="ES20"/>
+      <c r="ET20"/>
+      <c r="EU20"/>
+      <c r="EV20"/>
+      <c r="EW20"/>
+      <c r="EX20"/>
+      <c r="EY20"/>
+      <c r="EZ20"/>
+      <c r="FA20"/>
+      <c r="FB20"/>
+      <c r="FC20"/>
+      <c r="FD20"/>
+      <c r="FE20"/>
+      <c r="FF20"/>
+      <c r="FG20"/>
+      <c r="FH20"/>
+      <c r="FI20"/>
+      <c r="FJ20"/>
+      <c r="FK20"/>
+      <c r="FL20"/>
+      <c r="FM20"/>
+      <c r="FN20"/>
+      <c r="FO20"/>
+      <c r="FP20"/>
+      <c r="FQ20"/>
+      <c r="FR20"/>
+      <c r="FS20"/>
+      <c r="FT20"/>
+      <c r="FU20"/>
+      <c r="FV20"/>
+      <c r="FW20"/>
+      <c r="FX20"/>
+      <c r="FY20"/>
+      <c r="FZ20"/>
+      <c r="GA20"/>
+      <c r="GB20"/>
+      <c r="GC20"/>
+      <c r="GD20"/>
+      <c r="GE20"/>
+      <c r="GF20"/>
+      <c r="GG20"/>
+      <c r="GH20"/>
+      <c r="GI20"/>
+      <c r="GJ20"/>
+      <c r="GK20"/>
+      <c r="GL20"/>
+      <c r="GM20"/>
+      <c r="GN20"/>
+      <c r="GO20"/>
+      <c r="GP20"/>
+      <c r="GQ20"/>
+      <c r="GR20"/>
+      <c r="GS20"/>
+      <c r="GT20"/>
+      <c r="GU20"/>
+      <c r="GV20"/>
+      <c r="GW20"/>
+      <c r="GX20"/>
+      <c r="GY20"/>
+      <c r="GZ20"/>
+      <c r="HA20"/>
+      <c r="HB20"/>
+      <c r="HC20"/>
+      <c r="HD20"/>
+      <c r="HE20"/>
+      <c r="HF20"/>
+      <c r="HG20"/>
+      <c r="HH20"/>
+      <c r="HI20"/>
+      <c r="HJ20"/>
+      <c r="HK20"/>
+      <c r="HL20"/>
+      <c r="HM20"/>
+      <c r="HN20"/>
+      <c r="HO20"/>
+      <c r="HP20"/>
+      <c r="HQ20"/>
+      <c r="HR20"/>
+      <c r="HS20"/>
+      <c r="HT20"/>
+      <c r="HU20"/>
+      <c r="HV20"/>
+      <c r="HW20"/>
+      <c r="HX20"/>
+      <c r="HY20"/>
+      <c r="HZ20"/>
+      <c r="IA20"/>
+      <c r="IB20"/>
+      <c r="IC20"/>
+      <c r="ID20"/>
+      <c r="IE20"/>
+      <c r="IF20"/>
+      <c r="IG20"/>
+      <c r="IH20"/>
+      <c r="II20"/>
+      <c r="IJ20"/>
+      <c r="IK20"/>
+      <c r="IL20"/>
+      <c r="IM20"/>
+      <c r="IN20"/>
+      <c r="IO20"/>
+      <c r="IP20"/>
+      <c r="IQ20"/>
+      <c r="IR20"/>
+      <c r="IS20"/>
+      <c r="IT20"/>
+      <c r="IU20"/>
+      <c r="IV20"/>
+      <c r="IW20"/>
+      <c r="IX20"/>
+      <c r="IY20"/>
+      <c r="IZ20"/>
+      <c r="JA20"/>
+      <c r="JB20"/>
+      <c r="JC20"/>
+      <c r="JD20"/>
+      <c r="JE20"/>
+      <c r="JF20"/>
+      <c r="JG20"/>
+      <c r="JH20"/>
+      <c r="JI20"/>
+      <c r="JJ20"/>
+      <c r="JK20"/>
+      <c r="JL20"/>
+      <c r="JM20"/>
+      <c r="JN20"/>
+      <c r="JO20"/>
+      <c r="JP20"/>
+      <c r="JQ20"/>
+      <c r="JR20"/>
+      <c r="JS20"/>
+      <c r="JT20"/>
+      <c r="JU20"/>
+      <c r="JV20"/>
+      <c r="JW20"/>
+      <c r="JX20"/>
+      <c r="JY20"/>
+      <c r="JZ20"/>
+      <c r="KA20"/>
+      <c r="KB20"/>
+      <c r="KC20"/>
+      <c r="KD20"/>
+      <c r="KE20"/>
+      <c r="KF20"/>
+      <c r="KG20"/>
+      <c r="KH20"/>
+      <c r="KI20"/>
+      <c r="KJ20"/>
+      <c r="KK20"/>
+      <c r="KL20"/>
+      <c r="KM20"/>
+      <c r="KN20"/>
+      <c r="KO20"/>
+      <c r="KP20"/>
+      <c r="KQ20"/>
+      <c r="KR20"/>
+      <c r="KS20"/>
+      <c r="KT20"/>
+      <c r="KU20"/>
+      <c r="KV20"/>
+      <c r="KW20"/>
+      <c r="KX20"/>
+      <c r="KY20"/>
+      <c r="KZ20"/>
+      <c r="LA20"/>
+      <c r="LB20"/>
+      <c r="LC20"/>
+      <c r="LD20"/>
+      <c r="LE20"/>
+      <c r="LF20"/>
+      <c r="LG20"/>
+      <c r="LH20"/>
+      <c r="LI20"/>
+      <c r="LJ20"/>
+      <c r="LK20"/>
+      <c r="LL20"/>
+      <c r="LM20"/>
+      <c r="LN20"/>
+      <c r="LO20"/>
+      <c r="LP20"/>
+      <c r="LQ20"/>
+      <c r="LR20"/>
+      <c r="LS20"/>
+      <c r="LT20"/>
+      <c r="LU20"/>
+      <c r="LV20"/>
+      <c r="LW20"/>
+      <c r="LX20"/>
+      <c r="LY20"/>
+      <c r="LZ20"/>
+      <c r="MA20"/>
+      <c r="MB20"/>
+      <c r="MC20"/>
+      <c r="MD20"/>
+      <c r="ME20"/>
+      <c r="MF20"/>
+      <c r="MG20"/>
+      <c r="MH20"/>
+      <c r="MI20"/>
+      <c r="MJ20"/>
+      <c r="MK20"/>
+      <c r="ML20"/>
+      <c r="MM20"/>
+      <c r="MN20"/>
+      <c r="MO20"/>
+      <c r="MP20"/>
+      <c r="MQ20"/>
+      <c r="MR20"/>
+      <c r="MS20"/>
+      <c r="MT20"/>
+      <c r="MU20"/>
+      <c r="MV20"/>
+      <c r="MW20"/>
+      <c r="MX20"/>
+      <c r="MY20"/>
+      <c r="MZ20"/>
+      <c r="NA20"/>
+      <c r="NB20"/>
+    </row>
+    <row r="21" spans="1:366" x14ac:dyDescent="0.4">
+      <c r="A21" s="39"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="J21"/>
-      <c r="K21"/>
       <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21"/>
-      <c r="AJ21"/>
-      <c r="AK21"/>
-      <c r="AL21"/>
-      <c r="AM21"/>
-      <c r="AN21"/>
-      <c r="AO21"/>
-      <c r="AP21"/>
-      <c r="AQ21"/>
-      <c r="AR21"/>
-      <c r="AS21"/>
-      <c r="AT21"/>
-      <c r="AU21"/>
-      <c r="AV21"/>
-      <c r="AW21"/>
-      <c r="AX21"/>
-      <c r="AY21"/>
-      <c r="AZ21"/>
-      <c r="BA21"/>
-      <c r="BB21"/>
-      <c r="BC21"/>
-      <c r="BD21"/>
-      <c r="BE21"/>
-      <c r="BF21"/>
-      <c r="BG21"/>
-      <c r="BH21"/>
-      <c r="BI21"/>
-      <c r="BJ21"/>
-      <c r="BK21"/>
-      <c r="BL21"/>
-      <c r="BM21"/>
-      <c r="BN21"/>
-      <c r="BO21"/>
-      <c r="BP21"/>
-      <c r="BQ21"/>
-      <c r="BR21"/>
-      <c r="BS21"/>
-      <c r="BT21"/>
-      <c r="BU21"/>
-      <c r="BV21"/>
-      <c r="BW21"/>
-      <c r="BX21"/>
-      <c r="BY21"/>
-      <c r="BZ21"/>
-      <c r="CA21"/>
-      <c r="CB21"/>
-      <c r="CC21"/>
-      <c r="CD21"/>
-      <c r="CE21"/>
-      <c r="CF21"/>
-      <c r="CG21"/>
-      <c r="CH21"/>
-      <c r="CI21"/>
-      <c r="CJ21"/>
-      <c r="CK21"/>
-      <c r="CL21"/>
-      <c r="CM21"/>
-      <c r="CN21"/>
-      <c r="CO21"/>
-      <c r="CP21"/>
-      <c r="CQ21"/>
-      <c r="CR21"/>
-      <c r="CS21"/>
-      <c r="CT21"/>
-      <c r="CU21"/>
-      <c r="CV21"/>
-      <c r="CW21"/>
-      <c r="CX21"/>
-      <c r="CY21"/>
-      <c r="CZ21"/>
-      <c r="DA21"/>
-      <c r="DB21"/>
-      <c r="DC21"/>
-      <c r="DD21"/>
-      <c r="DE21"/>
-      <c r="DF21"/>
-      <c r="DG21"/>
-      <c r="DH21"/>
-      <c r="DI21"/>
-      <c r="DJ21"/>
-      <c r="DK21"/>
-      <c r="DL21"/>
-      <c r="DM21"/>
-      <c r="DN21"/>
-      <c r="DO21"/>
-      <c r="DP21"/>
-      <c r="DQ21"/>
-      <c r="DR21"/>
-      <c r="DS21"/>
-      <c r="DT21"/>
-      <c r="DU21"/>
-      <c r="DV21"/>
-      <c r="DW21"/>
-      <c r="DX21"/>
-      <c r="DY21"/>
-      <c r="DZ21"/>
-      <c r="EA21"/>
-      <c r="EB21"/>
-      <c r="EC21"/>
-      <c r="ED21"/>
-      <c r="EE21"/>
-      <c r="EF21"/>
-      <c r="EG21"/>
-      <c r="EH21"/>
-      <c r="EI21"/>
-      <c r="EJ21"/>
-      <c r="EK21"/>
-      <c r="EL21"/>
-      <c r="EM21"/>
-      <c r="EN21"/>
-      <c r="EO21"/>
-      <c r="EP21"/>
-      <c r="EQ21"/>
-      <c r="ER21"/>
-      <c r="ES21"/>
-      <c r="ET21"/>
-      <c r="EU21"/>
-      <c r="EV21"/>
-      <c r="EW21"/>
-      <c r="EX21"/>
-      <c r="EY21"/>
-      <c r="EZ21"/>
-      <c r="FA21"/>
-      <c r="FB21"/>
-      <c r="FC21"/>
-      <c r="FD21"/>
-      <c r="FE21"/>
-      <c r="FF21"/>
-      <c r="FG21"/>
-      <c r="FH21"/>
-      <c r="FI21"/>
-      <c r="FJ21"/>
-      <c r="FK21"/>
-      <c r="FL21"/>
-      <c r="FM21"/>
-      <c r="FN21"/>
-      <c r="FO21"/>
-      <c r="FP21"/>
-      <c r="FQ21"/>
-      <c r="FR21"/>
-      <c r="FS21"/>
-      <c r="FT21"/>
-      <c r="FU21"/>
-      <c r="FV21"/>
-      <c r="FW21"/>
-      <c r="FX21"/>
-      <c r="FY21"/>
-      <c r="FZ21"/>
-      <c r="GA21"/>
-      <c r="GB21"/>
-      <c r="GC21"/>
-      <c r="GD21"/>
-      <c r="GE21"/>
-      <c r="GF21"/>
-      <c r="GG21"/>
-      <c r="GH21"/>
-      <c r="GI21"/>
-      <c r="GJ21"/>
-      <c r="GK21"/>
-      <c r="GL21"/>
-      <c r="GM21"/>
-      <c r="GN21"/>
-      <c r="GO21"/>
-      <c r="GP21"/>
-      <c r="GQ21"/>
-      <c r="GR21"/>
-      <c r="GS21"/>
-      <c r="GT21"/>
-      <c r="GU21"/>
-      <c r="GV21"/>
-      <c r="GW21"/>
-      <c r="GX21"/>
-      <c r="GY21"/>
-      <c r="GZ21"/>
-      <c r="HA21"/>
-      <c r="HB21"/>
-      <c r="HC21"/>
-      <c r="HD21"/>
-      <c r="HE21"/>
-      <c r="HF21"/>
-      <c r="HG21"/>
-      <c r="HH21"/>
-      <c r="HI21"/>
-      <c r="HJ21"/>
-      <c r="HK21"/>
-      <c r="HL21"/>
-      <c r="HM21"/>
-      <c r="HN21"/>
-      <c r="HO21"/>
-      <c r="HP21"/>
-      <c r="HQ21"/>
-      <c r="HR21"/>
-      <c r="HS21"/>
-      <c r="HT21"/>
-      <c r="HU21"/>
-      <c r="HV21"/>
-      <c r="HW21"/>
-      <c r="HX21"/>
-      <c r="HY21"/>
-      <c r="HZ21"/>
-      <c r="IA21"/>
-      <c r="IB21"/>
-      <c r="IC21"/>
-      <c r="ID21"/>
-      <c r="IE21"/>
-      <c r="IF21"/>
-      <c r="IG21"/>
-      <c r="IH21"/>
-      <c r="II21"/>
-      <c r="IJ21"/>
-      <c r="IK21"/>
-      <c r="IL21"/>
-      <c r="IM21"/>
-      <c r="IN21"/>
-      <c r="IO21"/>
-      <c r="IP21"/>
-      <c r="IQ21"/>
-      <c r="IR21"/>
-      <c r="IS21"/>
-      <c r="IT21"/>
-      <c r="IU21"/>
-      <c r="IV21"/>
-      <c r="IW21"/>
-      <c r="IX21"/>
-      <c r="IY21"/>
-      <c r="IZ21"/>
-      <c r="JA21"/>
-      <c r="JB21"/>
-      <c r="JC21"/>
-      <c r="JD21"/>
-      <c r="JE21"/>
-      <c r="JF21"/>
-      <c r="JG21"/>
-      <c r="JH21"/>
-      <c r="JI21"/>
-      <c r="JJ21"/>
-      <c r="JK21"/>
-      <c r="JL21"/>
-      <c r="JM21"/>
-      <c r="JN21"/>
-      <c r="JO21"/>
-      <c r="JP21"/>
-      <c r="JQ21"/>
-      <c r="JR21"/>
-      <c r="JS21"/>
-      <c r="JT21"/>
-      <c r="JU21"/>
-      <c r="JV21"/>
-      <c r="JW21"/>
-      <c r="JX21"/>
-      <c r="JY21"/>
-      <c r="JZ21"/>
-      <c r="KA21"/>
-      <c r="KB21"/>
-      <c r="KC21"/>
-      <c r="KD21"/>
-      <c r="KE21"/>
-      <c r="KF21"/>
-      <c r="KG21"/>
-      <c r="KH21"/>
-      <c r="KI21"/>
-      <c r="KJ21"/>
-      <c r="KK21"/>
-      <c r="KL21"/>
-      <c r="KM21"/>
-      <c r="KN21"/>
-      <c r="KO21"/>
-      <c r="KP21"/>
-      <c r="KQ21"/>
-      <c r="KR21"/>
-      <c r="KS21"/>
-      <c r="KT21"/>
-      <c r="KU21"/>
-      <c r="KV21"/>
-      <c r="KW21"/>
-      <c r="KX21"/>
-      <c r="KY21"/>
-      <c r="KZ21"/>
-      <c r="LA21"/>
-      <c r="LB21"/>
-      <c r="LC21"/>
-      <c r="LD21"/>
-      <c r="LE21"/>
-      <c r="LF21"/>
-      <c r="LG21"/>
-      <c r="LH21"/>
-      <c r="LI21"/>
-      <c r="LJ21"/>
-      <c r="LK21"/>
-      <c r="LL21"/>
-      <c r="LM21"/>
-      <c r="LN21"/>
-      <c r="LO21"/>
-      <c r="LP21"/>
-      <c r="LQ21"/>
-      <c r="LR21"/>
-      <c r="LS21"/>
-      <c r="LT21"/>
-      <c r="LU21"/>
-      <c r="LV21"/>
-      <c r="LW21"/>
-      <c r="LX21"/>
-      <c r="LY21"/>
-      <c r="LZ21"/>
-      <c r="MA21"/>
-      <c r="MB21"/>
-      <c r="MC21"/>
-      <c r="MD21"/>
-      <c r="ME21"/>
-      <c r="MF21"/>
-      <c r="MG21"/>
-      <c r="MH21"/>
-      <c r="MI21"/>
-      <c r="MJ21"/>
-      <c r="MK21"/>
-      <c r="ML21"/>
-      <c r="MM21"/>
-      <c r="MN21"/>
-      <c r="MO21"/>
-      <c r="MP21"/>
-      <c r="MQ21"/>
-      <c r="MR21"/>
-      <c r="MS21"/>
-      <c r="MT21"/>
-      <c r="MU21"/>
-      <c r="MV21"/>
-      <c r="MW21"/>
-      <c r="MX21"/>
-      <c r="MY21"/>
-      <c r="MZ21"/>
-      <c r="NA21"/>
-      <c r="NB21"/>
     </row>
     <row r="22" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="22" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D22" s="28"/>
       <c r="J22"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="22" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D23" s="28"/>
       <c r="J23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
+    <row r="24" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="39"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="22" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D24" s="28"/>
+      <c r="E24" s="19"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
       <c r="J24"/>
+      <c r="K24"/>
       <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+      <c r="AT24"/>
+      <c r="AU24"/>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+      <c r="BA24"/>
+      <c r="BB24"/>
+      <c r="BC24"/>
+      <c r="BD24"/>
+      <c r="BE24"/>
+      <c r="BF24"/>
+      <c r="BG24"/>
+      <c r="BH24"/>
+      <c r="BI24"/>
+      <c r="BJ24"/>
+      <c r="BK24"/>
+      <c r="BL24"/>
+      <c r="BM24"/>
+      <c r="BN24"/>
+      <c r="BO24"/>
+      <c r="BP24"/>
+      <c r="BQ24"/>
+      <c r="BR24"/>
+      <c r="BS24"/>
+      <c r="BT24"/>
+      <c r="BU24"/>
+      <c r="BV24"/>
+      <c r="BW24"/>
+      <c r="BX24"/>
+      <c r="BY24"/>
+      <c r="BZ24"/>
+      <c r="CA24"/>
+      <c r="CB24"/>
+      <c r="CC24"/>
+      <c r="CD24"/>
+      <c r="CE24"/>
+      <c r="CF24"/>
+      <c r="CG24"/>
+      <c r="CH24"/>
+      <c r="CI24"/>
+      <c r="CJ24"/>
+      <c r="CK24"/>
+      <c r="CL24"/>
+      <c r="CM24"/>
+      <c r="CN24"/>
+      <c r="CO24"/>
+      <c r="CP24"/>
+      <c r="CQ24"/>
+      <c r="CR24"/>
+      <c r="CS24"/>
+      <c r="CT24"/>
+      <c r="CU24"/>
+      <c r="CV24"/>
+      <c r="CW24"/>
+      <c r="CX24"/>
+      <c r="CY24"/>
+      <c r="CZ24"/>
+      <c r="DA24"/>
+      <c r="DB24"/>
+      <c r="DC24"/>
+      <c r="DD24"/>
+      <c r="DE24"/>
+      <c r="DF24"/>
+      <c r="DG24"/>
+      <c r="DH24"/>
+      <c r="DI24"/>
+      <c r="DJ24"/>
+      <c r="DK24"/>
+      <c r="DL24"/>
+      <c r="DM24"/>
+      <c r="DN24"/>
+      <c r="DO24"/>
+      <c r="DP24"/>
+      <c r="DQ24"/>
+      <c r="DR24"/>
+      <c r="DS24"/>
+      <c r="DT24"/>
+      <c r="DU24"/>
+      <c r="DV24"/>
+      <c r="DW24"/>
+      <c r="DX24"/>
+      <c r="DY24"/>
+      <c r="DZ24"/>
+      <c r="EA24"/>
+      <c r="EB24"/>
+      <c r="EC24"/>
+      <c r="ED24"/>
+      <c r="EE24"/>
+      <c r="EF24"/>
+      <c r="EG24"/>
+      <c r="EH24"/>
+      <c r="EI24"/>
+      <c r="EJ24"/>
+      <c r="EK24"/>
+      <c r="EL24"/>
+      <c r="EM24"/>
+      <c r="EN24"/>
+      <c r="EO24"/>
+      <c r="EP24"/>
+      <c r="EQ24"/>
+      <c r="ER24"/>
+      <c r="ES24"/>
+      <c r="ET24"/>
+      <c r="EU24"/>
+      <c r="EV24"/>
+      <c r="EW24"/>
+      <c r="EX24"/>
+      <c r="EY24"/>
+      <c r="EZ24"/>
+      <c r="FA24"/>
+      <c r="FB24"/>
+      <c r="FC24"/>
+      <c r="FD24"/>
+      <c r="FE24"/>
+      <c r="FF24"/>
+      <c r="FG24"/>
+      <c r="FH24"/>
+      <c r="FI24"/>
+      <c r="FJ24"/>
+      <c r="FK24"/>
+      <c r="FL24"/>
+      <c r="FM24"/>
+      <c r="FN24"/>
+      <c r="FO24"/>
+      <c r="FP24"/>
+      <c r="FQ24"/>
+      <c r="FR24"/>
+      <c r="FS24"/>
+      <c r="FT24"/>
+      <c r="FU24"/>
+      <c r="FV24"/>
+      <c r="FW24"/>
+      <c r="FX24"/>
+      <c r="FY24"/>
+      <c r="FZ24"/>
+      <c r="GA24"/>
+      <c r="GB24"/>
+      <c r="GC24"/>
+      <c r="GD24"/>
+      <c r="GE24"/>
+      <c r="GF24"/>
+      <c r="GG24"/>
+      <c r="GH24"/>
+      <c r="GI24"/>
+      <c r="GJ24"/>
+      <c r="GK24"/>
+      <c r="GL24"/>
+      <c r="GM24"/>
+      <c r="GN24"/>
+      <c r="GO24"/>
+      <c r="GP24"/>
+      <c r="GQ24"/>
+      <c r="GR24"/>
+      <c r="GS24"/>
+      <c r="GT24"/>
+      <c r="GU24"/>
+      <c r="GV24"/>
+      <c r="GW24"/>
+      <c r="GX24"/>
+      <c r="GY24"/>
+      <c r="GZ24"/>
+      <c r="HA24"/>
+      <c r="HB24"/>
+      <c r="HC24"/>
+      <c r="HD24"/>
+      <c r="HE24"/>
+      <c r="HF24"/>
+      <c r="HG24"/>
+      <c r="HH24"/>
+      <c r="HI24"/>
+      <c r="HJ24"/>
+      <c r="HK24"/>
+      <c r="HL24"/>
+      <c r="HM24"/>
+      <c r="HN24"/>
+      <c r="HO24"/>
+      <c r="HP24"/>
+      <c r="HQ24"/>
+      <c r="HR24"/>
+      <c r="HS24"/>
+      <c r="HT24"/>
+      <c r="HU24"/>
+      <c r="HV24"/>
+      <c r="HW24"/>
+      <c r="HX24"/>
+      <c r="HY24"/>
+      <c r="HZ24"/>
+      <c r="IA24"/>
+      <c r="IB24"/>
+      <c r="IC24"/>
+      <c r="ID24"/>
+      <c r="IE24"/>
+      <c r="IF24"/>
+      <c r="IG24"/>
+      <c r="IH24"/>
+      <c r="II24"/>
+      <c r="IJ24"/>
+      <c r="IK24"/>
+      <c r="IL24"/>
+      <c r="IM24"/>
+      <c r="IN24"/>
+      <c r="IO24"/>
+      <c r="IP24"/>
+      <c r="IQ24"/>
+      <c r="IR24"/>
+      <c r="IS24"/>
+      <c r="IT24"/>
+      <c r="IU24"/>
+      <c r="IV24"/>
+      <c r="IW24"/>
+      <c r="IX24"/>
+      <c r="IY24"/>
+      <c r="IZ24"/>
+      <c r="JA24"/>
+      <c r="JB24"/>
+      <c r="JC24"/>
+      <c r="JD24"/>
+      <c r="JE24"/>
+      <c r="JF24"/>
+      <c r="JG24"/>
+      <c r="JH24"/>
+      <c r="JI24"/>
+      <c r="JJ24"/>
+      <c r="JK24"/>
+      <c r="JL24"/>
+      <c r="JM24"/>
+      <c r="JN24"/>
+      <c r="JO24"/>
+      <c r="JP24"/>
+      <c r="JQ24"/>
+      <c r="JR24"/>
+      <c r="JS24"/>
+      <c r="JT24"/>
+      <c r="JU24"/>
+      <c r="JV24"/>
+      <c r="JW24"/>
+      <c r="JX24"/>
+      <c r="JY24"/>
+      <c r="JZ24"/>
+      <c r="KA24"/>
+      <c r="KB24"/>
+      <c r="KC24"/>
+      <c r="KD24"/>
+      <c r="KE24"/>
+      <c r="KF24"/>
+      <c r="KG24"/>
+      <c r="KH24"/>
+      <c r="KI24"/>
+      <c r="KJ24"/>
+      <c r="KK24"/>
+      <c r="KL24"/>
+      <c r="KM24"/>
+      <c r="KN24"/>
+      <c r="KO24"/>
+      <c r="KP24"/>
+      <c r="KQ24"/>
+      <c r="KR24"/>
+      <c r="KS24"/>
+      <c r="KT24"/>
+      <c r="KU24"/>
+      <c r="KV24"/>
+      <c r="KW24"/>
+      <c r="KX24"/>
+      <c r="KY24"/>
+      <c r="KZ24"/>
+      <c r="LA24"/>
+      <c r="LB24"/>
+      <c r="LC24"/>
+      <c r="LD24"/>
+      <c r="LE24"/>
+      <c r="LF24"/>
+      <c r="LG24"/>
+      <c r="LH24"/>
+      <c r="LI24"/>
+      <c r="LJ24"/>
+      <c r="LK24"/>
+      <c r="LL24"/>
+      <c r="LM24"/>
+      <c r="LN24"/>
+      <c r="LO24"/>
+      <c r="LP24"/>
+      <c r="LQ24"/>
+      <c r="LR24"/>
+      <c r="LS24"/>
+      <c r="LT24"/>
+      <c r="LU24"/>
+      <c r="LV24"/>
+      <c r="LW24"/>
+      <c r="LX24"/>
+      <c r="LY24"/>
+      <c r="LZ24"/>
+      <c r="MA24"/>
+      <c r="MB24"/>
+      <c r="MC24"/>
+      <c r="MD24"/>
+      <c r="ME24"/>
+      <c r="MF24"/>
+      <c r="MG24"/>
+      <c r="MH24"/>
+      <c r="MI24"/>
+      <c r="MJ24"/>
+      <c r="MK24"/>
+      <c r="ML24"/>
+      <c r="MM24"/>
+      <c r="MN24"/>
+      <c r="MO24"/>
+      <c r="MP24"/>
+      <c r="MQ24"/>
+      <c r="MR24"/>
+      <c r="MS24"/>
+      <c r="MT24"/>
+      <c r="MU24"/>
+      <c r="MV24"/>
+      <c r="MW24"/>
+      <c r="MX24"/>
+      <c r="MY24"/>
+      <c r="MZ24"/>
+      <c r="NA24"/>
+      <c r="NB24"/>
     </row>
     <row r="25" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="26" t="s">
         <v>16</v>
       </c>
@@ -4892,10 +4918,10 @@
       <c r="NB25"/>
     </row>
     <row r="26" spans="1:366" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="36"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="20" t="s">
         <v>25</v>
       </c>
@@ -5264,10 +5290,10 @@
       <c r="NB26"/>
     </row>
     <row r="27" spans="1:366" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="26" t="s">
         <v>26</v>
       </c>
@@ -5636,10 +5662,10 @@
       <c r="NB27"/>
     </row>
     <row r="28" spans="1:366" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="38" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="20" t="s">
@@ -6010,8 +6036,8 @@
       <c r="NB28"/>
     </row>
     <row r="29" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="22" t="s">
         <v>34</v>
       </c>
@@ -6020,8 +6046,8 @@
       <c r="L29"/>
     </row>
     <row r="30" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="22" t="s">
         <v>35</v>
       </c>
@@ -6030,8 +6056,8 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="22" t="s">
         <v>36</v>
       </c>
@@ -6040,8 +6066,8 @@
       <c r="L31"/>
     </row>
     <row r="32" spans="1:366" x14ac:dyDescent="0.4">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="22" t="s">
         <v>39</v>
       </c>
@@ -6050,8 +6076,8 @@
       <c r="L32"/>
     </row>
     <row r="33" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="22" t="s">
         <v>46</v>
       </c>
@@ -6060,8 +6086,8 @@
       <c r="L33"/>
     </row>
     <row r="34" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="22" t="s">
         <v>52</v>
       </c>
@@ -6070,8 +6096,8 @@
       <c r="L34"/>
     </row>
     <row r="35" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="22" t="s">
         <v>53</v>
       </c>
@@ -6080,8 +6106,8 @@
       <c r="L35"/>
     </row>
     <row r="36" spans="1:80" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="26" t="s">
         <v>54</v>
       </c>
@@ -6164,8 +6190,8 @@
       <c r="CB36"/>
     </row>
     <row r="37" spans="1:80" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="33"/>
-      <c r="B37" s="32" t="s">
+      <c r="A37" s="39"/>
+      <c r="B37" s="38" t="s">
         <v>94</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -6250,8 +6276,8 @@
       <c r="CB37"/>
     </row>
     <row r="38" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="22" t="s">
         <v>70</v>
       </c>
@@ -6260,8 +6286,8 @@
       <c r="L38"/>
     </row>
     <row r="39" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="22" t="s">
         <v>76</v>
       </c>
@@ -6270,8 +6296,8 @@
       <c r="L39"/>
     </row>
     <row r="40" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="22" t="s">
         <v>32</v>
       </c>
@@ -6280,8 +6306,8 @@
       <c r="L40"/>
     </row>
     <row r="41" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="22" t="s">
         <v>33</v>
       </c>
@@ -6290,8 +6316,8 @@
       <c r="L41"/>
     </row>
     <row r="42" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="22" t="s">
         <v>50</v>
       </c>
@@ -6300,8 +6326,8 @@
       <c r="L42"/>
     </row>
     <row r="43" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="22" t="s">
         <v>37</v>
       </c>
@@ -6310,8 +6336,8 @@
       <c r="L43"/>
     </row>
     <row r="44" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="22" t="s">
         <v>40</v>
       </c>
@@ -6320,8 +6346,8 @@
       <c r="L44"/>
     </row>
     <row r="45" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="22" t="s">
         <v>49</v>
       </c>
@@ -6330,8 +6356,8 @@
       <c r="L45"/>
     </row>
     <row r="46" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="22" t="s">
         <v>79</v>
       </c>
@@ -6340,8 +6366,8 @@
       <c r="L46"/>
     </row>
     <row r="47" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A47" s="33"/>
-      <c r="B47" s="33"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
       <c r="C47" s="22" t="s">
         <v>83</v>
       </c>
@@ -6350,8 +6376,8 @@
       <c r="L47"/>
     </row>
     <row r="48" spans="1:80" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="33"/>
-      <c r="B48" s="34"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="40"/>
       <c r="C48" s="26" t="s">
         <v>56</v>
       </c>
@@ -6434,8 +6460,8 @@
       <c r="CB48"/>
     </row>
     <row r="49" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A49" s="33"/>
-      <c r="B49" s="32" t="s">
+      <c r="A49" s="39"/>
+      <c r="B49" s="38" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="22" t="s">
@@ -6446,8 +6472,8 @@
       <c r="L49"/>
     </row>
     <row r="50" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A50" s="33"/>
-      <c r="B50" s="33"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="22" t="s">
         <v>77</v>
       </c>
@@ -6456,8 +6482,8 @@
       <c r="L50"/>
     </row>
     <row r="51" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A51" s="33"/>
-      <c r="B51" s="33"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="22" t="s">
         <v>31</v>
       </c>
@@ -6466,8 +6492,8 @@
       <c r="L51"/>
     </row>
     <row r="52" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A52" s="33"/>
-      <c r="B52" s="33"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="22" t="s">
         <v>71</v>
       </c>
@@ -6476,8 +6502,8 @@
       <c r="L52"/>
     </row>
     <row r="53" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
       <c r="C53" s="22" t="s">
         <v>41</v>
       </c>
@@ -6486,8 +6512,8 @@
       <c r="L53"/>
     </row>
     <row r="54" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
       <c r="C54" s="22" t="s">
         <v>72</v>
       </c>
@@ -6496,8 +6522,8 @@
       <c r="L54"/>
     </row>
     <row r="55" spans="1:80" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="33"/>
-      <c r="B55" s="34"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="40"/>
       <c r="C55" s="22" t="s">
         <v>55</v>
       </c>
@@ -6506,8 +6532,8 @@
       <c r="L55"/>
     </row>
     <row r="56" spans="1:80" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="33"/>
-      <c r="B56" s="32" t="s">
+      <c r="A56" s="39"/>
+      <c r="B56" s="38" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="20" t="s">
@@ -6592,8 +6618,8 @@
       <c r="CB56"/>
     </row>
     <row r="57" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A57" s="33"/>
-      <c r="B57" s="33"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
       <c r="C57" s="22" t="s">
         <v>51</v>
       </c>
@@ -6602,8 +6628,8 @@
       <c r="L57"/>
     </row>
     <row r="58" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A58" s="33"/>
-      <c r="B58" s="33"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
       <c r="C58" s="22" t="s">
         <v>78</v>
       </c>
@@ -6612,8 +6638,8 @@
       <c r="L58"/>
     </row>
     <row r="59" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
       <c r="C59" s="22" t="s">
         <v>38</v>
       </c>
@@ -6622,8 +6648,8 @@
       <c r="L59"/>
     </row>
     <row r="60" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A60" s="33"/>
-      <c r="B60" s="33"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
       <c r="C60" s="22" t="s">
         <v>42</v>
       </c>
@@ -6632,8 +6658,8 @@
       <c r="L60"/>
     </row>
     <row r="61" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
       <c r="C61" s="22" t="s">
         <v>43</v>
       </c>
@@ -6642,8 +6668,8 @@
       <c r="L61"/>
     </row>
     <row r="62" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A62" s="33"/>
-      <c r="B62" s="33"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
       <c r="C62" s="22" t="s">
         <v>45</v>
       </c>
@@ -6652,8 +6678,8 @@
       <c r="L62"/>
     </row>
     <row r="63" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A63" s="33"/>
-      <c r="B63" s="33"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
       <c r="C63" s="22" t="s">
         <v>47</v>
       </c>
@@ -6662,8 +6688,8 @@
       <c r="L63"/>
     </row>
     <row r="64" spans="1:80" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="34"/>
-      <c r="B64" s="34"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="40"/>
       <c r="C64" s="26" t="s">
         <v>57</v>
       </c>
@@ -6746,10 +6772,10 @@
       <c r="CB64"/>
     </row>
     <row r="65" spans="1:80" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="32" t="s">
+      <c r="A65" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="38" t="s">
         <v>100</v>
       </c>
       <c r="C65" s="20" t="s">
@@ -6834,8 +6860,8 @@
       <c r="CB65"/>
     </row>
     <row r="66" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A66" s="33"/>
-      <c r="B66" s="33"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="39"/>
       <c r="C66" s="22" t="s">
         <v>59</v>
       </c>
@@ -6844,8 +6870,8 @@
       <c r="L66"/>
     </row>
     <row r="67" spans="1:80" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="33"/>
-      <c r="B67" s="34"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="40"/>
       <c r="C67" s="26" t="s">
         <v>60</v>
       </c>
@@ -6928,7 +6954,7 @@
       <c r="CB67"/>
     </row>
     <row r="68" spans="1:80" s="9" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="34"/>
+      <c r="A68" s="40"/>
       <c r="B68" s="9" t="s">
         <v>101</v>
       </c>
@@ -7014,7 +7040,7 @@
       <c r="CB68"/>
     </row>
     <row r="69" spans="1:80" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="38" t="s">
         <v>92</v>
       </c>
       <c r="B69" s="7" t="s">
@@ -7102,7 +7128,7 @@
       <c r="CB69"/>
     </row>
     <row r="70" spans="1:80" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="34"/>
+      <c r="A70" s="40"/>
       <c r="B70" t="s">
         <v>95</v>
       </c>
@@ -7114,7 +7140,7 @@
       <c r="L70"/>
     </row>
     <row r="71" spans="1:80" x14ac:dyDescent="0.4">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="38" t="s">
         <v>98</v>
       </c>
       <c r="B71" s="12" t="s">
@@ -7128,7 +7154,7 @@
       <c r="L71"/>
     </row>
     <row r="72" spans="1:80" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="34"/>
+      <c r="A72" s="40"/>
       <c r="B72" s="14" t="s">
         <v>94</v>
       </c>
@@ -18909,15 +18935,7 @@
       <c r="L2409"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:A25"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B21:B25"/>
+  <mergeCells count="18">
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="A69:A70"/>
@@ -18929,6 +18947,13 @@
     <mergeCell ref="B37:B48"/>
     <mergeCell ref="B49:B55"/>
     <mergeCell ref="B56:B64"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:A25"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18940,7 +18965,7 @@
   <dimension ref="A1:AE2409"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T64" sqref="T64"/>
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -18973,51 +18998,51 @@
       <c r="B1" s="41">
         <v>2</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="35">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="32">
         <v>3</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="41">
         <v>4</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="35" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="34"/>
       <c r="Q1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="35"/>
-      <c r="S1" s="36"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="34"/>
       <c r="T1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="34"/>
       <c r="W1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="35" t="s">
+      <c r="X1" s="32"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
       <c r="AC1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="36"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="34"/>
     </row>
     <row r="2" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
@@ -19667,33 +19692,39 @@
         <v>24</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11">
+      <c r="C11" s="43">
         <v>1</v>
       </c>
-      <c r="D11"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="2"/>
-      <c r="I11"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="1"/>
-      <c r="L11"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
       <c r="M11" s="2"/>
-      <c r="O11">
+      <c r="N11" s="43"/>
+      <c r="O11" s="43">
         <v>2</v>
       </c>
-      <c r="P11"/>
+      <c r="P11" s="43"/>
       <c r="Q11" s="1"/>
-      <c r="R11"/>
+      <c r="R11" s="43"/>
       <c r="S11" s="2">
         <v>2</v>
       </c>
-      <c r="U11">
+      <c r="T11" s="43"/>
+      <c r="U11" s="43">
         <v>2</v>
       </c>
-      <c r="V11"/>
+      <c r="V11" s="43"/>
       <c r="W11" s="1">
         <f>IF(Sheet1!$D11=1,Sheet2!N11,0)</f>
         <v>0</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="43">
         <f>IF(Sheet1!$D11=1,Sheet2!O11,0)</f>
         <v>0</v>
       </c>
@@ -19701,15 +19732,15 @@
         <f>IF(Sheet1!$D11=1,Sheet2!P11,0)</f>
         <v>0</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="43">
         <f>IF(Sheet1!$D11=1,Sheet2!Q11,0)</f>
         <v>0</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="43">
         <f>IF(Sheet1!$D11=1,Sheet2!R11,0)</f>
         <v>0</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="43">
         <f>IF(Sheet1!$D11=1,Sheet2!S11,0)</f>
         <v>0</v>
       </c>
@@ -19717,7 +19748,7 @@
         <f>IF(Sheet1!$D11=1,Sheet2!T11,0)</f>
         <v>0</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="43">
         <f>IF(Sheet1!$D11=1,Sheet2!U11,0)</f>
         <v>0</v>
       </c>
@@ -19731,32 +19762,39 @@
         <v>14</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12">
+      <c r="C12" s="43">
         <v>1</v>
       </c>
-      <c r="D12"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="2"/>
-      <c r="I12"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="1"/>
-      <c r="L12"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
       <c r="M12" s="2"/>
-      <c r="P12">
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43">
         <v>2</v>
       </c>
       <c r="Q12" s="1">
         <v>2</v>
       </c>
-      <c r="R12"/>
+      <c r="R12" s="43"/>
       <c r="S12" s="2"/>
-      <c r="T12">
+      <c r="T12" s="43">
         <v>2</v>
       </c>
-      <c r="V12"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
       <c r="W12" s="1">
         <f>IF(Sheet1!$D12=1,Sheet2!N12,0)</f>
         <v>0</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="43">
         <f>IF(Sheet1!$D12=1,Sheet2!O12,0)</f>
         <v>0</v>
       </c>
@@ -19764,15 +19802,15 @@
         <f>IF(Sheet1!$D12=1,Sheet2!P12,0)</f>
         <v>0</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="43">
         <f>IF(Sheet1!$D12=1,Sheet2!Q12,0)</f>
         <v>0</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="43">
         <f>IF(Sheet1!$D12=1,Sheet2!R12,0)</f>
         <v>0</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="43">
         <f>IF(Sheet1!$D12=1,Sheet2!S12,0)</f>
         <v>0</v>
       </c>
@@ -19780,7 +19818,7 @@
         <f>IF(Sheet1!$D12=1,Sheet2!T12,0)</f>
         <v>0</v>
       </c>
-      <c r="AD12">
+      <c r="AD12" s="43">
         <f>IF(Sheet1!$D12=1,Sheet2!U12,0)</f>
         <v>0</v>
       </c>
@@ -19789,142 +19827,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A13" s="22" t="s">
+    <row r="13" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13">
+      <c r="B13" s="3"/>
+      <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13"/>
-      <c r="E13" s="2"/>
-      <c r="I13"/>
-      <c r="J13" s="1"/>
-      <c r="L13"/>
-      <c r="M13" s="2"/>
-      <c r="P13">
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5">
         <v>2</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="3">
         <v>2</v>
       </c>
-      <c r="R13"/>
-      <c r="S13" s="2"/>
-      <c r="U13">
+      <c r="R13" s="5"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5">
         <v>2</v>
       </c>
-      <c r="V13"/>
-      <c r="W13" s="1">
+      <c r="V13" s="5"/>
+      <c r="W13" s="3">
         <f>IF(Sheet1!$D13=1,Sheet2!N13,0)</f>
         <v>0</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="5">
         <f>IF(Sheet1!$D13=1,Sheet2!O13,0)</f>
         <v>0</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Y13" s="4">
         <f>IF(Sheet1!$D13=1,Sheet2!P13,0)</f>
         <v>0</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="5">
         <f>IF(Sheet1!$D13=1,Sheet2!Q13,0)</f>
         <v>0</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="5">
         <f>IF(Sheet1!$D13=1,Sheet2!R13,0)</f>
         <v>0</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="5">
         <f>IF(Sheet1!$D13=1,Sheet2!S13,0)</f>
         <v>0</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AC13" s="3">
         <f>IF(Sheet1!$D13=1,Sheet2!T13,0)</f>
         <v>0</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="5">
         <f>IF(Sheet1!$D13=1,Sheet2!U13,0)</f>
         <v>0</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AE13" s="4">
         <f>IF(Sheet1!$D13=1,Sheet2!V13,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5">
+      <c r="E14" s="2"/>
+      <c r="I14"/>
+      <c r="J14" s="1"/>
+      <c r="L14"/>
+      <c r="M14" s="2"/>
+      <c r="N14">
         <v>2</v>
       </c>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="5">
+      <c r="P14"/>
+      <c r="Q14" s="1"/>
+      <c r="R14"/>
+      <c r="S14" s="2">
         <v>2</v>
       </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5">
+      <c r="U14">
         <v>2</v>
       </c>
-      <c r="W14" s="3">
+      <c r="V14"/>
+      <c r="W14" s="1">
         <f>IF(Sheet1!$D14=1,Sheet2!N14,0)</f>
         <v>0</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14">
         <f>IF(Sheet1!$D14=1,Sheet2!O14,0)</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="4">
+      <c r="Y14" s="2">
         <f>IF(Sheet1!$D14=1,Sheet2!P14,0)</f>
         <v>0</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14">
         <f>IF(Sheet1!$D14=1,Sheet2!Q14,0)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="5">
+      <c r="AA14">
         <f>IF(Sheet1!$D14=1,Sheet2!R14,0)</f>
         <v>0</v>
       </c>
-      <c r="AB14" s="5">
+      <c r="AB14">
         <f>IF(Sheet1!$D14=1,Sheet2!S14,0)</f>
         <v>0</v>
       </c>
-      <c r="AC14" s="3">
+      <c r="AC14" s="1">
         <f>IF(Sheet1!$D14=1,Sheet2!T14,0)</f>
         <v>0</v>
       </c>
-      <c r="AD14" s="5">
+      <c r="AD14">
         <f>IF(Sheet1!$D14=1,Sheet2!U14,0)</f>
         <v>0</v>
       </c>
-      <c r="AE14" s="4">
+      <c r="AE14" s="2">
         <f>IF(Sheet1!$D14=1,Sheet2!V14,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1"/>
       <c r="D15">
@@ -19940,11 +19978,11 @@
       </c>
       <c r="P15"/>
       <c r="Q15" s="1"/>
-      <c r="R15"/>
-      <c r="S15" s="2">
+      <c r="R15">
         <v>2</v>
       </c>
-      <c r="U15">
+      <c r="S15" s="2"/>
+      <c r="T15">
         <v>2</v>
       </c>
       <c r="V15"/>
@@ -19987,7 +20025,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1"/>
       <c r="D16">
@@ -19998,16 +20036,16 @@
       <c r="J16" s="1"/>
       <c r="L16"/>
       <c r="M16" s="2"/>
-      <c r="N16">
+      <c r="O16">
         <v>2</v>
       </c>
       <c r="P16"/>
       <c r="Q16" s="1"/>
-      <c r="R16">
+      <c r="R16"/>
+      <c r="S16" s="2">
         <v>2</v>
       </c>
-      <c r="S16" s="2"/>
-      <c r="T16">
+      <c r="U16">
         <v>2</v>
       </c>
       <c r="V16"/>
@@ -20050,7 +20088,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1"/>
       <c r="D17">
@@ -20066,10 +20104,10 @@
       </c>
       <c r="P17"/>
       <c r="Q17" s="1"/>
-      <c r="R17"/>
-      <c r="S17" s="2">
+      <c r="R17">
         <v>2</v>
       </c>
+      <c r="S17" s="2"/>
       <c r="U17">
         <v>2</v>
       </c>
@@ -20113,7 +20151,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1"/>
       <c r="D18">
@@ -20124,10 +20162,9 @@
       <c r="J18" s="1"/>
       <c r="L18"/>
       <c r="M18" s="2"/>
-      <c r="O18">
+      <c r="P18">
         <v>2</v>
       </c>
-      <c r="P18"/>
       <c r="Q18" s="1"/>
       <c r="R18">
         <v>2</v>
@@ -20174,9 +20211,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="22" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1"/>
       <c r="D19">
@@ -20191,10 +20228,10 @@
         <v>2</v>
       </c>
       <c r="Q19" s="1"/>
-      <c r="R19">
+      <c r="R19"/>
+      <c r="S19" s="2">
         <v>2</v>
       </c>
-      <c r="S19" s="2"/>
       <c r="U19">
         <v>2</v>
       </c>
@@ -20236,160 +20273,165 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="D20">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A20" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="I20"/>
-      <c r="J20" s="1"/>
-      <c r="L20"/>
-      <c r="M20" s="2"/>
-      <c r="P20">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7">
         <v>2</v>
       </c>
-      <c r="Q20" s="1"/>
-      <c r="R20"/>
-      <c r="S20" s="2">
+      <c r="P20" s="7"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="7">
         <v>2</v>
       </c>
-      <c r="U20">
+      <c r="S20" s="8"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7">
         <v>2</v>
       </c>
-      <c r="V20"/>
-      <c r="W20" s="1">
+      <c r="V20" s="7"/>
+      <c r="W20" s="6">
         <f>IF(Sheet1!$D20=1,Sheet2!N20,0)</f>
         <v>0</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="7">
         <f>IF(Sheet1!$D20=1,Sheet2!O20,0)</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Y20" s="8">
         <f>IF(Sheet1!$D20=1,Sheet2!P20,0)</f>
         <v>0</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="7">
         <f>IF(Sheet1!$D20=1,Sheet2!Q20,0)</f>
         <v>0</v>
       </c>
-      <c r="AA20">
+      <c r="AA20" s="7">
         <f>IF(Sheet1!$D20=1,Sheet2!R20,0)</f>
         <v>0</v>
       </c>
-      <c r="AB20">
+      <c r="AB20" s="7">
         <f>IF(Sheet1!$D20=1,Sheet2!S20,0)</f>
         <v>0</v>
       </c>
-      <c r="AC20" s="1">
+      <c r="AC20" s="6">
         <f>IF(Sheet1!$D20=1,Sheet2!T20,0)</f>
         <v>0</v>
       </c>
-      <c r="AD20">
+      <c r="AD20" s="7">
         <f>IF(Sheet1!$D20=1,Sheet2!U20,0)</f>
         <v>0</v>
       </c>
-      <c r="AE20" s="2">
+      <c r="AE20" s="8">
         <f>IF(Sheet1!$D20=1,Sheet2!V20,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8">
+      <c r="A21" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7">
+      <c r="I21"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="2"/>
+      <c r="O21">
         <v>2</v>
       </c>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="7">
+      <c r="P21"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="2">
         <v>2</v>
       </c>
-      <c r="S21" s="8"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7">
+      <c r="U21">
         <v>2</v>
       </c>
-      <c r="V21" s="7"/>
-      <c r="W21" s="6">
+      <c r="V21"/>
+      <c r="W21" s="1">
         <f>IF(Sheet1!$D21=1,Sheet2!N21,0)</f>
         <v>0</v>
       </c>
-      <c r="X21" s="7">
+      <c r="X21" s="43">
         <f>IF(Sheet1!$D21=1,Sheet2!O21,0)</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="8">
+      <c r="Y21" s="2">
         <f>IF(Sheet1!$D21=1,Sheet2!P21,0)</f>
         <v>0</v>
       </c>
-      <c r="Z21" s="7">
+      <c r="Z21">
         <f>IF(Sheet1!$D21=1,Sheet2!Q21,0)</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="7">
+      <c r="AA21">
         <f>IF(Sheet1!$D21=1,Sheet2!R21,0)</f>
         <v>0</v>
       </c>
-      <c r="AB21" s="7">
+      <c r="AB21">
         <f>IF(Sheet1!$D21=1,Sheet2!S21,0)</f>
         <v>0</v>
       </c>
-      <c r="AC21" s="6">
+      <c r="AC21" s="1">
         <f>IF(Sheet1!$D21=1,Sheet2!T21,0)</f>
         <v>0</v>
       </c>
-      <c r="AD21" s="7">
+      <c r="AD21" s="43">
         <f>IF(Sheet1!$D21=1,Sheet2!U21,0)</f>
         <v>0</v>
       </c>
-      <c r="AE21" s="8">
+      <c r="AE21" s="2">
         <f>IF(Sheet1!$D21=1,Sheet2!V21,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A22" s="22" t="s">
-        <v>22</v>
+      <c r="A22" s="45" t="s">
+        <v>17</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="D22"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="2">
         <v>1</v>
       </c>
       <c r="I22"/>
       <c r="J22" s="1"/>
-      <c r="L22"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
       <c r="M22" s="2"/>
       <c r="O22">
         <v>2</v>
       </c>
       <c r="P22"/>
       <c r="Q22" s="1"/>
-      <c r="R22"/>
-      <c r="S22" s="2">
+      <c r="R22" s="43">
         <v>2</v>
       </c>
+      <c r="S22" s="2"/>
       <c r="U22">
         <v>2</v>
       </c>
@@ -20398,7 +20440,7 @@
         <f>IF(Sheet1!$D22=1,Sheet2!N22,0)</f>
         <v>0</v>
       </c>
-      <c r="X22">
+      <c r="X22" s="43">
         <f>IF(Sheet1!$D22=1,Sheet2!O22,0)</f>
         <v>0</v>
       </c>
@@ -20422,7 +20464,7 @@
         <f>IF(Sheet1!$D22=1,Sheet2!T22,0)</f>
         <v>0</v>
       </c>
-      <c r="AD22">
+      <c r="AD22" s="43">
         <f>IF(Sheet1!$D22=1,Sheet2!U22,0)</f>
         <v>0</v>
       </c>
@@ -20432,27 +20474,29 @@
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A23" s="22" t="s">
-        <v>17</v>
+      <c r="A23" s="45" t="s">
+        <v>23</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="D23"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2">
         <v>1</v>
       </c>
       <c r="I23"/>
       <c r="J23" s="1"/>
-      <c r="L23"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
       <c r="M23" s="2"/>
       <c r="O23">
         <v>2</v>
       </c>
       <c r="P23"/>
       <c r="Q23" s="1"/>
-      <c r="R23">
+      <c r="R23" s="43"/>
+      <c r="S23" s="2">
         <v>2</v>
       </c>
-      <c r="S23" s="2"/>
       <c r="U23">
         <v>2</v>
       </c>
@@ -20461,7 +20505,7 @@
         <f>IF(Sheet1!$D23=1,Sheet2!N23,0)</f>
         <v>0</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="43">
         <f>IF(Sheet1!$D23=1,Sheet2!O23,0)</f>
         <v>0</v>
       </c>
@@ -20485,7 +20529,7 @@
         <f>IF(Sheet1!$D23=1,Sheet2!T23,0)</f>
         <v>0</v>
       </c>
-      <c r="AD23">
+      <c r="AD23" s="43">
         <f>IF(Sheet1!$D23=1,Sheet2!U23,0)</f>
         <v>0</v>
       </c>
@@ -20495,36 +20539,43 @@
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A24" s="22" t="s">
-        <v>23</v>
+      <c r="A24" s="42" t="s">
+        <v>81</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="D24"/>
-      <c r="E24" s="2">
+      <c r="C24" s="43">
         <v>1</v>
       </c>
-      <c r="I24"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
       <c r="J24" s="1"/>
-      <c r="L24"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
       <c r="M24" s="2"/>
-      <c r="O24">
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43">
         <v>2</v>
       </c>
-      <c r="P24"/>
       <c r="Q24" s="1"/>
-      <c r="R24"/>
-      <c r="S24" s="2">
+      <c r="R24" s="43">
         <v>2</v>
       </c>
-      <c r="U24">
+      <c r="S24" s="2"/>
+      <c r="T24" s="43"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="43">
         <v>2</v>
       </c>
-      <c r="V24"/>
       <c r="W24" s="1">
         <f>IF(Sheet1!$D24=1,Sheet2!N24,0)</f>
         <v>0</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="43">
         <f>IF(Sheet1!$D24=1,Sheet2!O24,0)</f>
         <v>0</v>
       </c>
@@ -20532,15 +20583,15 @@
         <f>IF(Sheet1!$D24=1,Sheet2!P24,0)</f>
         <v>0</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="43">
         <f>IF(Sheet1!$D24=1,Sheet2!Q24,0)</f>
         <v>0</v>
       </c>
-      <c r="AA24">
+      <c r="AA24" s="43">
         <f>IF(Sheet1!$D24=1,Sheet2!R24,0)</f>
         <v>0</v>
       </c>
-      <c r="AB24">
+      <c r="AB24" s="43">
         <f>IF(Sheet1!$D24=1,Sheet2!S24,0)</f>
         <v>0</v>
       </c>
@@ -20548,7 +20599,7 @@
         <f>IF(Sheet1!$D24=1,Sheet2!T24,0)</f>
         <v>0</v>
       </c>
-      <c r="AD24">
+      <c r="AD24" s="43">
         <f>IF(Sheet1!$D24=1,Sheet2!U24,0)</f>
         <v>0</v>
       </c>
@@ -20558,7 +20609,7 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3"/>

</xml_diff>